<commit_message>
add: validate import user and student topic
</commit_message>
<xml_diff>
--- a/public/init_data/student_topic_init.xlsx
+++ b/public/init_data/student_topic_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HTTT\DoAnTN\Project\FE3\public\init_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2983F8EB-8221-4671-9D39-E7884D5E96A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F15173-1384-41B3-8CD8-BCFF645D82D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,7 +512,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +520,7 @@
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.77734375" customWidth="1"/>
     <col min="7" max="7" width="32.77734375" customWidth="1"/>
   </cols>
@@ -537,7 +538,7 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
@@ -560,7 +561,7 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
@@ -583,7 +584,7 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F3" t="s">
@@ -606,7 +607,7 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
@@ -629,7 +630,7 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
@@ -652,7 +653,7 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F6" t="s">

</xml_diff>